<commit_message>
Removed rows with all Na values
</commit_message>
<xml_diff>
--- a/Python/Data/Final/bone_marrow.xlsx
+++ b/Python/Data/Final/bone_marrow.xlsx
@@ -1226,7 +1226,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1240,19 +1240,19 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>